<commit_message>
Results by meat type and MRIO folder with only the needed stuff
</commit_message>
<xml_diff>
--- a/MRIO/Inputs/Support information for MRIO/Extensions.xlsx
+++ b/MRIO/Inputs/Support information for MRIO/Extensions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gollinucci\Documents\GitHub\MEAT_SSA\MRIO\Inputs\Support information for MRIO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FC4F906-065A-4B22-B48B-399E5BA53067}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD6A9914-3EE3-4A31-B8B8-70637097E0D2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-5445" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,15 +36,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
   <si>
-    <t>GHG: GWP_100</t>
-  </si>
-  <si>
-    <t>EUT</t>
-  </si>
-  <si>
-    <t>Fossil Fuels (from ton to GJ)</t>
-  </si>
-  <si>
     <t>Anthracite</t>
   </si>
   <si>
@@ -154,13 +145,22 @@
   </si>
   <si>
     <t>Eutrophication</t>
+  </si>
+  <si>
+    <t>University of Leiden, 1992</t>
+  </si>
+  <si>
+    <t>Energy statistics handbook (from ton to GJ)</t>
+  </si>
+  <si>
+    <t>Low bound GWP_100</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,6 +172,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -198,9 +204,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -485,620 +494,621 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="14.109375" customWidth="1"/>
-    <col min="5" max="5" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" t="s">
-        <v>1</v>
+        <v>22</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>2</v>
+        <v>38</v>
       </c>
       <c r="G2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
         <v>21</v>
-      </c>
-      <c r="F3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
+        <v>8</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2">
         <v>41.9</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
+        <v>9</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2">
         <v>53.83</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2">
         <v>27.7</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0</v>
+      </c>
+      <c r="F10" s="2">
         <v>28.8</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0</v>
+      </c>
+      <c r="F11" s="2">
         <v>15</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
+        <v>3</v>
+      </c>
+      <c r="B12" s="2">
+        <v>0</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0</v>
+      </c>
+      <c r="F12" s="2">
         <v>29</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
+        <v>4</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0</v>
+      </c>
+      <c r="F13" s="2">
         <v>18.3</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
+        <v>10</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0</v>
+      </c>
+      <c r="G14" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15">
+        <v>11</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0</v>
+      </c>
+      <c r="G15" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16">
+        <v>12</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0</v>
+      </c>
+      <c r="G16" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-      <c r="G17">
+        <v>13</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0</v>
+      </c>
+      <c r="G17" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18">
+        <v>31</v>
+      </c>
+      <c r="B18" s="2">
         <v>1</v>
       </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="G18">
+      <c r="C18" s="2">
+        <v>0</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0</v>
+      </c>
+      <c r="G18" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19">
+        <v>29</v>
+      </c>
+      <c r="B19" s="2">
         <v>265</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="2">
         <v>265</v>
       </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="G19">
+      <c r="D19" s="2">
+        <v>0</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0</v>
+      </c>
+      <c r="G19" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>33</v>
-      </c>
-      <c r="B20">
+        <v>30</v>
+      </c>
+      <c r="B20" s="2">
         <v>28</v>
       </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20">
+      <c r="C20" s="2">
+        <v>0</v>
+      </c>
+      <c r="D20" s="2">
         <v>28</v>
       </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-      <c r="G20">
+      <c r="E20" s="2">
+        <v>0</v>
+      </c>
+      <c r="F20" s="2">
+        <v>0</v>
+      </c>
+      <c r="G20" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>35</v>
-      </c>
-      <c r="B21">
+        <v>32</v>
+      </c>
+      <c r="B21" s="2">
         <v>1</v>
       </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="G21">
+      <c r="C21" s="2">
+        <v>0</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0</v>
+      </c>
+      <c r="F21" s="2">
+        <v>0</v>
+      </c>
+      <c r="G21" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>36</v>
-      </c>
-      <c r="B22">
-        <v>0</v>
-      </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22">
+        <v>33</v>
+      </c>
+      <c r="B22" s="2">
+        <v>0</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0</v>
+      </c>
+      <c r="E22" s="2">
         <v>0.13</v>
       </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
-      <c r="G22">
+      <c r="F22" s="2">
+        <v>0</v>
+      </c>
+      <c r="G22" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>28</v>
-      </c>
-      <c r="B23">
-        <v>0</v>
-      </c>
-      <c r="C23">
-        <v>0</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
+        <v>25</v>
+      </c>
+      <c r="B23" s="2">
+        <v>0</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0</v>
+      </c>
+      <c r="E23" s="2">
         <v>0.42</v>
       </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-      <c r="G23">
+      <c r="F23" s="2">
+        <v>0</v>
+      </c>
+      <c r="G23" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>29</v>
-      </c>
-      <c r="B24">
-        <v>0</v>
-      </c>
-      <c r="C24">
-        <v>0</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24">
+        <v>26</v>
+      </c>
+      <c r="B24" s="2">
+        <v>0</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0</v>
+      </c>
+      <c r="E24" s="2">
         <v>3.07</v>
       </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
-      <c r="G24">
+      <c r="F24" s="2">
+        <v>0</v>
+      </c>
+      <c r="G24" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>30</v>
-      </c>
-      <c r="B25">
-        <v>0</v>
-      </c>
-      <c r="C25">
-        <v>0</v>
-      </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25">
-        <v>0</v>
-      </c>
-      <c r="F25">
-        <v>0</v>
-      </c>
-      <c r="G25">
+        <v>27</v>
+      </c>
+      <c r="B25" s="2">
+        <v>0</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0</v>
+      </c>
+      <c r="F25" s="2">
+        <v>0</v>
+      </c>
+      <c r="G25" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>31</v>
-      </c>
-      <c r="B26">
-        <v>0</v>
-      </c>
-      <c r="C26">
-        <v>0</v>
-      </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26">
+        <v>28</v>
+      </c>
+      <c r="B26" s="2">
+        <v>0</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0</v>
+      </c>
+      <c r="E26" s="2">
         <v>0.35</v>
       </c>
-      <c r="F26">
-        <v>0</v>
-      </c>
-      <c r="G26">
+      <c r="F26" s="2">
+        <v>0</v>
+      </c>
+      <c r="G26" s="2">
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" display="Fossil Fuels (from ton to EJ]" xr:uid="{E41919EE-5AF0-46B4-A4DD-B6A47081E0E4}"/>
+    <hyperlink ref="E2" r:id="rId2" display="EUT" xr:uid="{20A7C856-0F0F-4F15-B0DB-59C4F1931F0E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>